<commit_message>
publications & collections complete
</commit_message>
<xml_diff>
--- a/AppreciationApp/DataStructure.xlsx
+++ b/AppreciationApp/DataStructure.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timurozkul/Documents/Repo/Others/AppreciationApp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timurozkul/Documents/Repo/Mini-projects/AppreciationApp/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24160" windowHeight="12100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27560" windowHeight="15060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>UserId</t>
   </si>
@@ -38,37 +38,46 @@
     <t>Users Collection</t>
   </si>
   <si>
+    <t>Message Collection</t>
+  </si>
+  <si>
+    <t>messageId</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>messages [ str ]</t>
+  </si>
+  <si>
+    <t>dayScore - int</t>
+  </si>
+  <si>
+    <t>points - int</t>
+  </si>
+  <si>
+    <t>sport - str</t>
+  </si>
+  <si>
+    <t>subjects [ { } ]</t>
+  </si>
+  <si>
+    <t>Day Collection</t>
+  </si>
+  <si>
     <t>date</t>
   </si>
   <si>
-    <t>appr [ { } ]</t>
-  </si>
-  <si>
-    <t>fields [ { } ]</t>
-  </si>
-  <si>
-    <t>Message Collection</t>
-  </si>
-  <si>
-    <t>messageId</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>messages [ str ]</t>
-  </si>
-  <si>
-    <t>dayScore - int</t>
-  </si>
-  <si>
-    <t>dayMessage - str</t>
-  </si>
-  <si>
-    <t>points - int</t>
-  </si>
-  <si>
-    <t>sport - str</t>
+    <t>feedback - str</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currentSubjects [ { } ] </t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>daysGoal</t>
   </si>
 </sst>
 </file>
@@ -92,7 +101,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,12 +116,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -126,6 +129,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -151,15 +166,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,21 +453,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -472,65 +490,88 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C6" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="10" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="19" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C6" s="2" t="s">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C8" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="13" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
+      <c r="B21" s="3" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>